<commit_message>
Update county impact download link
</commit_message>
<xml_diff>
--- a/Forecast/TCs_within_50_miles_1851-2019.xlsx
+++ b/Forecast/TCs_within_50_miles_1851-2019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Phils_Work_Files\Landfalling_Hurricanes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmbell/Development/csu-tropical/Forecast/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC07B647-2CDA-43E2-A184-6678B31A367A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D42096-7D30-D84C-93AB-F502C61F68CD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="County" sheetId="1" r:id="rId1"/>
@@ -19,16 +19,6 @@
     <sheet name="Caribbean-Central America" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -876,25 +866,25 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="30.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="30.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="13.25" style="2" customWidth="1"/>
-    <col min="9" max="9" width="20.125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="7.625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="41.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="20.1640625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="7.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="41.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="26" width="7.625" style="1" customWidth="1"/>
-    <col min="27" max="16384" width="12.625" style="1"/>
+    <col min="14" max="26" width="7.6640625" style="1" customWidth="1"/>
+    <col min="27" max="16384" width="12.6640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -902,10 +892,10 @@
         <v>179</v>
       </c>
       <c r="B1" s="1">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H2" s="11" t="s">
         <v>180</v>
       </c>
@@ -915,7 +905,7 @@
       </c>
       <c r="M2" s="4"/>
     </row>
-    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B3" s="5"/>
       <c r="C3" s="6" t="s">
         <v>128</v>
@@ -935,7 +925,7 @@
       </c>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
@@ -970,7 +960,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>6</v>
       </c>
@@ -1000,18 +990,18 @@
       </c>
       <c r="K5" s="12">
         <f>(1-(1/(2.71828^((C5*($B$1/100))/169))))</f>
-        <v>0.27779306535378978</v>
+        <v>0.34069416798360319</v>
       </c>
       <c r="L5" s="12">
-        <f t="shared" ref="L5:M5" si="1">(1-(1/(2.71828^((D5*($B$1/100))/169))))</f>
-        <v>0.15643492295654537</v>
+        <f t="shared" ref="L5" si="1">(1-(1/(2.71828^((D5*($B$1/100))/169))))</f>
+        <v>0.19567457386278631</v>
       </c>
       <c r="M5" s="4">
         <f>IF(E5*($B$1/100)&gt;0, (1-(1/(2.71828^(E5*($B$1/100)/169)))), "&lt;1%")</f>
-        <v>5.7454945699552895E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+        <v>7.2942413534695993E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
@@ -1041,18 +1031,18 @@
       </c>
       <c r="K6" s="12">
         <f t="shared" ref="K6:K69" si="4">(1-(1/(2.71828^((C6*($B$1/100))/169))))</f>
-        <v>0.25610678982041879</v>
+        <v>0.3152476028782849</v>
       </c>
       <c r="L6" s="12">
         <f t="shared" ref="L6:L69" si="5">(1-(1/(2.71828^((D6*($B$1/100))/169))))</f>
-        <v>0.15017240886976957</v>
+        <v>0.18802350279309388</v>
       </c>
       <c r="M6" s="4">
         <f t="shared" ref="M6:M69" si="6">IF(E6*($B$1/100)&gt;0, (1-(1/(2.71828^(E6*($B$1/100)/169)))), "&lt;1%")</f>
-        <v>6.4400709453971694E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+        <v>8.1677867706266838E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1082,18 +1072,18 @@
       </c>
       <c r="K7" s="12">
         <f t="shared" si="4"/>
-        <v>0.28839796079267044</v>
+        <v>0.35306060886918966</v>
       </c>
       <c r="L7" s="12">
         <f t="shared" si="5"/>
-        <v>0.1749469262936646</v>
+        <v>0.21819793210070104</v>
       </c>
       <c r="M7" s="4">
         <f t="shared" si="6"/>
-        <v>8.4932400084761439E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+        <v>0.10739345208458406</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1123,18 +1113,18 @@
       </c>
       <c r="K8" s="12">
         <f t="shared" si="4"/>
-        <v>0.26158865667956688</v>
+        <v>0.32169986999875255</v>
       </c>
       <c r="L8" s="12">
         <f t="shared" si="5"/>
-        <v>0.16265128758536473</v>
+        <v>0.20325355061852413</v>
       </c>
       <c r="M8" s="4">
         <f t="shared" si="6"/>
-        <v>6.4400709453971694E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+        <v>8.1677867706266838E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -1164,18 +1154,18 @@
       </c>
       <c r="K9" s="12">
         <f t="shared" si="4"/>
-        <v>0.25058422631632693</v>
+        <v>0.30873395916484248</v>
       </c>
       <c r="L9" s="12">
         <f t="shared" si="5"/>
-        <v>0.15643492295654537</v>
+        <v>0.19567457386278631</v>
       </c>
       <c r="M9" s="4">
         <f t="shared" si="6"/>
-        <v>6.4400709453971694E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+        <v>8.1677867706266838E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -1205,18 +1195,18 @@
       </c>
       <c r="K10" s="12">
         <f t="shared" si="4"/>
-        <v>0.27243149785310483</v>
+        <v>0.33442258236228806</v>
       </c>
       <c r="L10" s="12">
         <f t="shared" si="5"/>
-        <v>0.16882184283889112</v>
+        <v>0.21076111238873818</v>
       </c>
       <c r="M10" s="4">
         <f t="shared" si="6"/>
-        <v>7.1295288775442778E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+        <v>9.0331009666926976E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -1246,18 +1236,18 @@
       </c>
       <c r="K11" s="12">
         <f t="shared" si="4"/>
-        <v>0.23941579862461304</v>
+        <v>0.29552020104870858</v>
       </c>
       <c r="L11" s="12">
         <f t="shared" si="5"/>
-        <v>0.14386340271764586</v>
+        <v>0.18029965161896699</v>
       </c>
       <c r="M11" s="4">
         <f t="shared" si="6"/>
-        <v>5.7454945699552895E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+        <v>7.2942413534695993E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
@@ -1287,18 +1277,18 @@
       </c>
       <c r="K12" s="12">
         <f t="shared" si="4"/>
-        <v>0.29364186889971078</v>
+        <v>0.35915657257793254</v>
       </c>
       <c r="L12" s="12">
         <f t="shared" si="5"/>
-        <v>0.16265128758536473</v>
+        <v>0.20325355061852413</v>
       </c>
       <c r="M12" s="4">
         <f t="shared" si="6"/>
-        <v>5.7454945699552895E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+        <v>7.2942413534695993E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
@@ -1328,18 +1318,18 @@
       </c>
       <c r="K13" s="12">
         <f t="shared" si="4"/>
-        <v>0.36312579829540614</v>
+        <v>0.43870822152458266</v>
       </c>
       <c r="L13" s="12">
         <f t="shared" si="5"/>
-        <v>0.20490190865211622</v>
+        <v>0.2543440117125576</v>
       </c>
       <c r="M13" s="4">
         <f t="shared" si="6"/>
-        <v>7.8139060850156983E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+        <v>9.8902615026041585E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -1369,18 +1359,18 @@
       </c>
       <c r="K14" s="12">
         <f t="shared" si="4"/>
-        <v>0.34883602988775952</v>
+        <v>0.42253766337222631</v>
       </c>
       <c r="L14" s="12">
         <f t="shared" si="5"/>
-        <v>0.1930526844259034</v>
+        <v>0.24009057340511064</v>
       </c>
       <c r="M14" s="4">
         <f t="shared" si="6"/>
-        <v>5.0457617525815013E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+        <v>6.4123864164936761E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -1410,18 +1400,18 @@
       </c>
       <c r="K15" s="12">
         <f t="shared" si="4"/>
-        <v>0.38624862043206354</v>
+        <v>0.46465915993124107</v>
       </c>
       <c r="L15" s="12">
         <f t="shared" si="5"/>
-        <v>0.21657713872523698</v>
+        <v>0.26833010170654215</v>
       </c>
       <c r="M15" s="4">
         <f t="shared" si="6"/>
-        <v>5.7454945699552895E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+        <v>7.2942413534695993E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
@@ -1451,18 +1441,18 @@
       </c>
       <c r="K16" s="12">
         <f t="shared" si="4"/>
-        <v>0.33422563696651553</v>
+        <v>0.40590123887194485</v>
       </c>
       <c r="L16" s="12">
         <f t="shared" si="5"/>
-        <v>0.16882184283889112</v>
+        <v>0.21076111238873818</v>
       </c>
       <c r="M16" s="4">
         <f t="shared" si="6"/>
-        <v>5.0457617525815013E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+        <v>6.4123864164936761E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
@@ -1492,18 +1482,18 @@
       </c>
       <c r="K17" s="12">
         <f t="shared" si="4"/>
-        <v>0.31423390663665962</v>
+        <v>0.38297140559897314</v>
       </c>
       <c r="L17" s="12">
         <f t="shared" si="5"/>
-        <v>0.16882184283889112</v>
+        <v>0.21076111238873818</v>
       </c>
       <c r="M17" s="4">
         <f t="shared" si="6"/>
-        <v>2.9152404184648928E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+        <v>3.7161702846576494E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
@@ -1533,18 +1523,18 @@
       </c>
       <c r="K18" s="12">
         <f t="shared" si="4"/>
-        <v>0.35363456029344487</v>
+        <v>0.4279789604945049</v>
       </c>
       <c r="L18" s="12">
         <f t="shared" si="5"/>
-        <v>0.18102687303857068</v>
+        <v>0.22556467634084354</v>
       </c>
       <c r="M18" s="4">
         <f t="shared" si="6"/>
-        <v>5.0457617525815013E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+        <v>6.4123864164936761E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -1574,18 +1564,18 @@
       </c>
       <c r="K19" s="12">
         <f t="shared" si="4"/>
-        <v>0.35363456029344487</v>
+        <v>0.4279789604945049</v>
       </c>
       <c r="L19" s="12">
         <f t="shared" si="5"/>
-        <v>0.1870620156931716</v>
+        <v>0.23286200541450353</v>
       </c>
       <c r="M19" s="4">
         <f t="shared" si="6"/>
-        <v>6.4400709453971694E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+        <v>8.1677867706266838E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
@@ -1615,18 +1605,18 @@
       </c>
       <c r="K20" s="12">
         <f t="shared" si="4"/>
-        <v>0.39077145153385251</v>
+        <v>0.4697035557086614</v>
       </c>
       <c r="L20" s="12">
         <f t="shared" si="5"/>
-        <v>0.1930526844259034</v>
+        <v>0.24009057340511064</v>
       </c>
       <c r="M20" s="4">
         <f t="shared" si="6"/>
-        <v>7.1295288775442778E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+        <v>9.0331009666926976E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -1656,18 +1646,18 @@
       </c>
       <c r="K21" s="12">
         <f t="shared" si="4"/>
-        <v>0.39526095317707544</v>
+        <v>0.47470041928443607</v>
       </c>
       <c r="L21" s="12">
         <f t="shared" si="5"/>
-        <v>0.20490190865211622</v>
+        <v>0.2543440117125576</v>
       </c>
       <c r="M21" s="4">
         <f t="shared" si="6"/>
-        <v>6.4400709453971694E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+        <v>8.1677867706266838E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -1697,18 +1687,18 @@
       </c>
       <c r="K22" s="12">
         <f t="shared" si="4"/>
-        <v>0.48986325937563424</v>
+        <v>0.57748819089125425</v>
       </c>
       <c r="L22" s="12">
         <f t="shared" si="5"/>
-        <v>0.26158865667956688</v>
+        <v>0.32169986999875255</v>
       </c>
       <c r="M22" s="4">
         <f t="shared" si="6"/>
-        <v>9.1675678126840299E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+        <v>0.11580428190400116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
@@ -1738,15 +1728,15 @@
       </c>
       <c r="K23" s="12">
         <f t="shared" si="4"/>
-        <v>0.46671420723255974</v>
+        <v>0.55279276843269742</v>
       </c>
       <c r="L23" s="12">
         <f t="shared" si="5"/>
-        <v>0.26158865667956688</v>
+        <v>0.32169986999875255</v>
       </c>
       <c r="M23" s="4">
         <f t="shared" si="6"/>
-        <v>9.1675678126840299E-2</v>
+        <v>0.11580428190400116</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1779,15 +1769,15 @@
       </c>
       <c r="K24" s="12">
         <f t="shared" si="4"/>
-        <v>0.45070081538434603</v>
+        <v>0.53553236001367477</v>
       </c>
       <c r="L24" s="12">
         <f t="shared" si="5"/>
-        <v>0.23376932343862444</v>
+        <v>0.28881890225373608</v>
       </c>
       <c r="M24" s="4">
         <f t="shared" si="6"/>
-        <v>8.4932400084761439E-2</v>
+        <v>0.10739345208458406</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1820,15 +1810,15 @@
       </c>
       <c r="K25" s="12">
         <f t="shared" si="4"/>
-        <v>0.50838465824413892</v>
+        <v>0.59702273309326026</v>
       </c>
       <c r="L25" s="12">
         <f t="shared" si="5"/>
-        <v>0.27243149785310483</v>
+        <v>0.33442258236228806</v>
       </c>
       <c r="M25" s="4">
         <f t="shared" si="6"/>
-        <v>9.8369263885248692E-2</v>
+        <v>0.12413585837442997</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1861,15 +1851,15 @@
       </c>
       <c r="K26" s="12">
         <f t="shared" si="4"/>
-        <v>0.46671420723255974</v>
+        <v>0.55279276843269742</v>
       </c>
       <c r="L26" s="12">
         <f t="shared" si="5"/>
-        <v>0.25610678982041879</v>
+        <v>0.3152476028782849</v>
       </c>
       <c r="M26" s="4">
         <f t="shared" si="6"/>
-        <v>9.8369263885248692E-2</v>
+        <v>0.12413585837442997</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1902,15 +1892,15 @@
       </c>
       <c r="K27" s="12">
         <f t="shared" si="4"/>
-        <v>0.37247766684275874</v>
+        <v>0.44923623638659793</v>
       </c>
       <c r="L27" s="12">
         <f t="shared" si="5"/>
-        <v>0.1749469262936646</v>
+        <v>0.21819793210070104</v>
       </c>
       <c r="M27" s="4">
         <f t="shared" si="6"/>
-        <v>6.4400709453971694E-2</v>
+        <v>8.1677867706266838E-2</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1943,15 +1933,15 @@
       </c>
       <c r="K28" s="12">
         <f t="shared" si="4"/>
-        <v>0.40853192841956476</v>
+        <v>0.48941027459201225</v>
       </c>
       <c r="L28" s="12">
         <f t="shared" si="5"/>
-        <v>0.21657713872523698</v>
+        <v>0.26833010170654215</v>
       </c>
       <c r="M28" s="4">
         <f t="shared" si="6"/>
-        <v>6.4400709453971694E-2</v>
+        <v>8.1677867706266838E-2</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1984,15 +1974,15 @@
       </c>
       <c r="K29" s="12">
         <f t="shared" si="4"/>
-        <v>0.39526095317707544</v>
+        <v>0.47470041928443607</v>
       </c>
       <c r="L29" s="12">
         <f t="shared" si="5"/>
-        <v>0.1989992069721388</v>
+        <v>0.24725102823281386</v>
       </c>
       <c r="M29" s="4">
         <f t="shared" si="6"/>
-        <v>7.8139060850156983E-2</v>
+        <v>9.8902615026041585E-2</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2025,15 +2015,15 @@
       </c>
       <c r="K30" s="12">
         <f t="shared" si="4"/>
-        <v>0.44251469435523794</v>
+        <v>0.52665392148928847</v>
       </c>
       <c r="L30" s="12">
         <f t="shared" si="5"/>
-        <v>0.22235030584271132</v>
+        <v>0.27522446183969218</v>
       </c>
       <c r="M30" s="4">
         <f t="shared" si="6"/>
-        <v>7.8139060850156983E-2</v>
+        <v>9.8902615026041585E-2</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2066,15 +2056,15 @@
       </c>
       <c r="K31" s="12">
         <f t="shared" si="4"/>
-        <v>0.45070081538434603</v>
+        <v>0.53553236001367477</v>
       </c>
       <c r="L31" s="12">
         <f t="shared" si="5"/>
-        <v>0.21076111238873818</v>
+        <v>0.26137015961160848</v>
       </c>
       <c r="M31" s="4">
         <f t="shared" si="6"/>
-        <v>7.8139060850156983E-2</v>
+        <v>9.8902615026041585E-2</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2107,15 +2097,15 @@
       </c>
       <c r="K32" s="12">
         <f t="shared" si="4"/>
-        <v>0.44251469435523794</v>
+        <v>0.52665392148928847</v>
       </c>
       <c r="L32" s="12">
         <f t="shared" si="5"/>
-        <v>0.21076111238873818</v>
+        <v>0.26137015961160848</v>
       </c>
       <c r="M32" s="4">
         <f t="shared" si="6"/>
-        <v>7.8139060850156983E-2</v>
+        <v>9.8902615026041585E-2</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2148,15 +2138,15 @@
       </c>
       <c r="K33" s="12">
         <f t="shared" si="4"/>
-        <v>0.4041409487181139</v>
+        <v>0.48455333715151305</v>
       </c>
       <c r="L33" s="12">
         <f t="shared" si="5"/>
-        <v>0.1989992069721388</v>
+        <v>0.24725102823281386</v>
       </c>
       <c r="M33" s="4">
         <f t="shared" si="6"/>
-        <v>6.4400709453971694E-2</v>
+        <v>8.1677867706266838E-2</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2189,15 +2179,15 @@
       </c>
       <c r="K34" s="12">
         <f t="shared" si="4"/>
-        <v>0.41721705279824384</v>
+        <v>0.49898728324175334</v>
       </c>
       <c r="L34" s="12">
         <f t="shared" si="5"/>
-        <v>0.1989992069721388</v>
+        <v>0.24725102823281386</v>
       </c>
       <c r="M34" s="4">
         <f t="shared" si="6"/>
-        <v>6.4400709453971694E-2</v>
+        <v>8.1677867706266838E-2</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2230,15 +2220,15 @@
       </c>
       <c r="K35" s="12">
         <f t="shared" si="4"/>
-        <v>0.42151167261816491</v>
+        <v>0.50370821286954803</v>
       </c>
       <c r="L35" s="12">
         <f t="shared" si="5"/>
-        <v>0.21076111238873818</v>
+        <v>0.26137015961160848</v>
       </c>
       <c r="M35" s="4">
         <f t="shared" si="6"/>
-        <v>7.1295288775442778E-2</v>
+        <v>9.0331009666926976E-2</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2271,15 +2261,15 @@
       </c>
       <c r="K36" s="12">
         <f t="shared" si="4"/>
-        <v>0.43000620227468589</v>
+        <v>0.51301703853059311</v>
       </c>
       <c r="L36" s="12">
         <f t="shared" si="5"/>
-        <v>0.22808092957753268</v>
+        <v>0.28205385797506577</v>
       </c>
       <c r="M36" s="4">
         <f t="shared" si="6"/>
-        <v>6.4400709453971694E-2</v>
+        <v>8.1677867706266838E-2</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2312,15 +2302,15 @@
       </c>
       <c r="K37" s="12">
         <f t="shared" si="4"/>
-        <v>0.44662289184871728</v>
+        <v>0.53111415463606493</v>
       </c>
       <c r="L37" s="12">
         <f t="shared" si="5"/>
-        <v>0.21657713872523698</v>
+        <v>0.26833010170654215</v>
       </c>
       <c r="M37" s="4">
         <f t="shared" si="6"/>
-        <v>4.340834212541933E-2</v>
+        <v>5.5221429161617874E-2</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2353,15 +2343,15 @@
       </c>
       <c r="K38" s="12">
         <f t="shared" si="4"/>
-        <v>0.44251469435523794</v>
+        <v>0.52665392148928847</v>
       </c>
       <c r="L38" s="12">
         <f t="shared" si="5"/>
-        <v>0.20490190865211622</v>
+        <v>0.2543440117125576</v>
       </c>
       <c r="M38" s="4">
         <f t="shared" si="6"/>
-        <v>4.340834212541933E-2</v>
+        <v>5.5221429161617874E-2</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2394,15 +2384,15 @@
       </c>
       <c r="K39" s="12">
         <f t="shared" si="4"/>
-        <v>0.39971737097178972</v>
+        <v>0.47965019854376145</v>
       </c>
       <c r="L39" s="12">
         <f t="shared" si="5"/>
-        <v>0.18102687303857068</v>
+        <v>0.22556467634084354</v>
       </c>
       <c r="M39" s="4">
         <f t="shared" si="6"/>
-        <v>2.9152404184648928E-2</v>
+        <v>3.7161702846576494E-2</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2435,15 +2425,15 @@
       </c>
       <c r="K40" s="12">
         <f t="shared" si="4"/>
-        <v>0.39971737097178972</v>
+        <v>0.47965019854376145</v>
       </c>
       <c r="L40" s="12">
         <f t="shared" si="5"/>
-        <v>0.14386340271764586</v>
+        <v>0.18029965161896699</v>
       </c>
       <c r="M40" s="4">
         <f t="shared" si="6"/>
-        <v>7.3691583471030553E-3</v>
+        <v>9.4227740532037974E-3</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2476,15 +2466,15 @@
       </c>
       <c r="K41" s="12">
         <f t="shared" si="4"/>
-        <v>0.40853192841956476</v>
+        <v>0.48941027459201225</v>
       </c>
       <c r="L41" s="12">
         <f t="shared" si="5"/>
-        <v>0.16265128758536473</v>
+        <v>0.20325355061852413</v>
       </c>
       <c r="M41" s="4">
         <f t="shared" si="6"/>
-        <v>1.4684012199461582E-2</v>
+        <v>1.8756759435549886E-2</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2517,15 +2507,15 @@
       </c>
       <c r="K42" s="12">
         <f t="shared" si="4"/>
-        <v>0.40853192841956476</v>
+        <v>0.48941027459201225</v>
       </c>
       <c r="L42" s="12">
         <f t="shared" si="5"/>
-        <v>0.16265128758536473</v>
+        <v>0.20325355061852413</v>
       </c>
       <c r="M42" s="4">
         <f t="shared" si="6"/>
-        <v>1.4684012199461582E-2</v>
+        <v>1.8756759435549886E-2</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2558,15 +2548,15 @@
       </c>
       <c r="K43" s="12">
         <f t="shared" si="4"/>
-        <v>0.41289055029629673</v>
+        <v>0.49422144620841901</v>
       </c>
       <c r="L43" s="12">
         <f t="shared" si="5"/>
-        <v>0.1870620156931716</v>
+        <v>0.23286200541450353</v>
       </c>
       <c r="M43" s="4">
         <f t="shared" si="6"/>
-        <v>2.9152404184648928E-2</v>
+        <v>3.7161702846576494E-2</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2599,15 +2589,15 @@
       </c>
       <c r="K44" s="12">
         <f t="shared" si="4"/>
-        <v>0.41721705279824384</v>
+        <v>0.49898728324175334</v>
       </c>
       <c r="L44" s="12">
         <f t="shared" si="5"/>
-        <v>0.22235030584271132</v>
+        <v>0.27522446183969218</v>
       </c>
       <c r="M44" s="4">
         <f t="shared" si="6"/>
-        <v>2.9152404184648928E-2</v>
+        <v>3.7161702846576494E-2</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2640,15 +2630,15 @@
       </c>
       <c r="K45" s="12">
         <f t="shared" si="4"/>
-        <v>0.4041409487181139</v>
+        <v>0.48455333715151305</v>
       </c>
       <c r="L45" s="12">
         <f t="shared" si="5"/>
-        <v>0.21657713872523698</v>
+        <v>0.26833010170654215</v>
       </c>
       <c r="M45" s="4">
         <f t="shared" si="6"/>
-        <v>4.340834212541933E-2</v>
+        <v>5.5221429161617874E-2</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2681,15 +2671,15 @@
       </c>
       <c r="K46" s="12">
         <f t="shared" si="4"/>
-        <v>0.41721705279824384</v>
+        <v>0.49898728324175334</v>
       </c>
       <c r="L46" s="12">
         <f t="shared" si="5"/>
-        <v>0.21076111238873818</v>
+        <v>0.26137015961160848</v>
       </c>
       <c r="M46" s="4">
         <f t="shared" si="6"/>
-        <v>5.0457617525815013E-2</v>
+        <v>6.4123864164936761E-2</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2722,15 +2712,15 @@
       </c>
       <c r="K47" s="12">
         <f t="shared" si="4"/>
-        <v>0.42151167261816491</v>
+        <v>0.50370821286954803</v>
       </c>
       <c r="L47" s="12">
         <f t="shared" si="5"/>
-        <v>0.20490190865211622</v>
+        <v>0.2543440117125576</v>
       </c>
       <c r="M47" s="4">
         <f t="shared" si="6"/>
-        <v>7.1295288775442778E-2</v>
+        <v>9.0331009666926976E-2</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2763,15 +2753,15 @@
       </c>
       <c r="K48" s="12">
         <f t="shared" si="4"/>
-        <v>0.43837599815410178</v>
+        <v>0.52215126078808638</v>
       </c>
       <c r="L48" s="12">
         <f t="shared" si="5"/>
-        <v>0.22235030584271132</v>
+        <v>0.27522446183969218</v>
       </c>
       <c r="M48" s="4">
         <f t="shared" si="6"/>
-        <v>8.4932400084761439E-2</v>
+        <v>0.10739345208458406</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2804,15 +2794,15 @@
       </c>
       <c r="K49" s="12">
         <f t="shared" si="4"/>
-        <v>0.43000620227468589</v>
+        <v>0.51301703853059311</v>
       </c>
       <c r="L49" s="12">
         <f t="shared" si="5"/>
-        <v>0.1989992069721388</v>
+        <v>0.24725102823281386</v>
       </c>
       <c r="M49" s="4">
         <f t="shared" si="6"/>
-        <v>9.1675678126840299E-2</v>
+        <v>0.11580428190400116</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2845,15 +2835,15 @@
       </c>
       <c r="K50" s="12">
         <f t="shared" si="4"/>
-        <v>0.44251469435523794</v>
+        <v>0.52665392148928847</v>
       </c>
       <c r="L50" s="12">
         <f t="shared" si="5"/>
-        <v>0.20490190865211622</v>
+        <v>0.2543440117125576</v>
       </c>
       <c r="M50" s="4">
         <f t="shared" si="6"/>
-        <v>0.11160882061376709</v>
+        <v>0.14056423137712515</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2886,15 +2876,15 @@
       </c>
       <c r="K51" s="12">
         <f t="shared" si="4"/>
-        <v>0.46275516497207569</v>
+        <v>0.54853875109044536</v>
       </c>
       <c r="L51" s="12">
         <f t="shared" si="5"/>
-        <v>0.21076111238873818</v>
+        <v>0.26137015961160848</v>
       </c>
       <c r="M51" s="4">
         <f t="shared" si="6"/>
-        <v>0.13110453105155007</v>
+        <v>0.16463083311584525</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2927,15 +2917,15 @@
       </c>
       <c r="K52" s="12">
         <f t="shared" si="4"/>
-        <v>0.48986325937563424</v>
+        <v>0.57748819089125425</v>
       </c>
       <c r="L52" s="12">
         <f t="shared" si="5"/>
-        <v>0.25610678982041879</v>
+        <v>0.3152476028782849</v>
       </c>
       <c r="M52" s="4">
         <f t="shared" si="6"/>
-        <v>0.14386340271764586</v>
+        <v>0.18029965161896699</v>
       </c>
     </row>
     <row r="53" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2968,15 +2958,15 @@
       </c>
       <c r="K53" s="12">
         <f t="shared" si="4"/>
-        <v>0.60034721501867783</v>
+        <v>0.69086082760161927</v>
       </c>
       <c r="L53" s="12">
         <f t="shared" si="5"/>
-        <v>0.35839772956873728</v>
+        <v>0.43336898550344394</v>
       </c>
       <c r="M53" s="4">
         <f t="shared" si="6"/>
-        <v>0.1749469262936646</v>
+        <v>0.21819793210070104</v>
       </c>
     </row>
     <row r="54" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3009,15 +2999,15 @@
       </c>
       <c r="K54" s="12">
         <f t="shared" si="4"/>
-        <v>0.50105819062850654</v>
+        <v>0.5893197015299374</v>
       </c>
       <c r="L54" s="12">
         <f t="shared" si="5"/>
-        <v>0.27779306535378978</v>
+        <v>0.34069416798360319</v>
       </c>
       <c r="M54" s="4">
         <f t="shared" si="6"/>
-        <v>0.15017240886976957</v>
+        <v>0.18802350279309388</v>
       </c>
     </row>
     <row r="55" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3050,15 +3040,15 @@
       </c>
       <c r="K55" s="12">
         <f t="shared" si="4"/>
-        <v>0.50105819062850654</v>
+        <v>0.5893197015299374</v>
       </c>
       <c r="L55" s="12">
         <f t="shared" si="5"/>
-        <v>0.27243149785310483</v>
+        <v>0.33442258236228806</v>
       </c>
       <c r="M55" s="4">
         <f t="shared" si="6"/>
-        <v>0.12465396752976854</v>
+        <v>0.15668446133949132</v>
       </c>
     </row>
     <row r="56" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3091,15 +3081,15 @@
       </c>
       <c r="K56" s="12">
         <f t="shared" si="4"/>
-        <v>0.50838465824413892</v>
+        <v>0.59702273309326026</v>
       </c>
       <c r="L56" s="12">
         <f t="shared" si="5"/>
-        <v>0.26703012679379212</v>
+        <v>0.32809133886401298</v>
       </c>
       <c r="M56" s="4">
         <f t="shared" si="6"/>
-        <v>0.11160882061376709</v>
+        <v>0.14056423137712515</v>
       </c>
     </row>
     <row r="57" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3132,15 +3122,15 @@
       </c>
       <c r="K57" s="12">
         <f t="shared" si="4"/>
-        <v>0.46671420723255974</v>
+        <v>0.55279276843269742</v>
       </c>
       <c r="L57" s="12">
         <f t="shared" si="5"/>
-        <v>0.22808092957753268</v>
+        <v>0.28205385797506577</v>
       </c>
       <c r="M57" s="4">
         <f t="shared" si="6"/>
-        <v>9.1675678126840299E-2</v>
+        <v>0.11580428190400116</v>
       </c>
     </row>
     <row r="58" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3173,15 +3163,15 @@
       </c>
       <c r="K58" s="12">
         <f t="shared" si="4"/>
-        <v>0.44662289184871728</v>
+        <v>0.53111415463606493</v>
       </c>
       <c r="L58" s="12">
         <f t="shared" si="5"/>
-        <v>0.21076111238873818</v>
+        <v>0.26137015961160848</v>
       </c>
       <c r="M58" s="4">
         <f t="shared" si="6"/>
-        <v>7.8139060850156983E-2</v>
+        <v>9.8902615026041585E-2</v>
       </c>
     </row>
     <row r="59" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3214,15 +3204,15 @@
       </c>
       <c r="K59" s="12">
         <f t="shared" si="4"/>
-        <v>0.45070081538434603</v>
+        <v>0.53553236001367477</v>
       </c>
       <c r="L59" s="12">
         <f t="shared" si="5"/>
-        <v>0.22235030584271132</v>
+        <v>0.27522446183969218</v>
       </c>
       <c r="M59" s="4">
         <f t="shared" si="6"/>
-        <v>8.4932400084761439E-2</v>
+        <v>0.10739345208458406</v>
       </c>
     </row>
     <row r="60" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3255,15 +3245,15 @@
       </c>
       <c r="K60" s="12">
         <f t="shared" si="4"/>
-        <v>0.49735411349835601</v>
+        <v>0.585413143253386</v>
       </c>
       <c r="L60" s="12">
         <f t="shared" si="5"/>
-        <v>0.21657713872523698</v>
+        <v>0.26833010170654215</v>
       </c>
       <c r="M60" s="4">
         <f t="shared" si="6"/>
-        <v>7.1295288775442778E-2</v>
+        <v>9.0331009666926976E-2</v>
       </c>
     </row>
     <row r="61" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3296,15 +3286,15 @@
       </c>
       <c r="K61" s="12">
         <f t="shared" si="4"/>
-        <v>0.47064407468372338</v>
+        <v>0.55700670113071471</v>
       </c>
       <c r="L61" s="12">
         <f t="shared" si="5"/>
-        <v>0.21657713872523698</v>
+        <v>0.26833010170654215</v>
       </c>
       <c r="M61" s="4">
         <f t="shared" si="6"/>
-        <v>3.6306733849116646E-2</v>
+        <v>4.6234310570424819E-2</v>
       </c>
     </row>
     <row r="62" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3337,15 +3327,15 @@
       </c>
       <c r="K62" s="12">
         <f t="shared" si="4"/>
-        <v>0.42577464470459248</v>
+        <v>0.50838465824413892</v>
       </c>
       <c r="L62" s="12">
         <f t="shared" si="5"/>
-        <v>0.1870620156931716</v>
+        <v>0.23286200541450353</v>
       </c>
       <c r="M62" s="4">
         <f t="shared" si="6"/>
-        <v>3.6306733849116646E-2</v>
+        <v>4.6234310570424819E-2</v>
       </c>
     </row>
     <row r="63" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3378,15 +3368,15 @@
       </c>
       <c r="K63" s="12">
         <f t="shared" si="4"/>
-        <v>0.45474868805571345</v>
+        <v>0.5399089336402908</v>
       </c>
       <c r="L63" s="12">
         <f t="shared" si="5"/>
-        <v>0.18102687303857068</v>
+        <v>0.22556467634084354</v>
       </c>
       <c r="M63" s="4">
         <f t="shared" si="6"/>
-        <v>5.0457617525815013E-2</v>
+        <v>6.4123864164936761E-2</v>
       </c>
     </row>
     <row r="64" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3419,15 +3409,15 @@
       </c>
       <c r="K64" s="12">
         <f t="shared" si="4"/>
-        <v>0.46275516497207569</v>
+        <v>0.54853875109044536</v>
       </c>
       <c r="L64" s="12">
         <f t="shared" si="5"/>
-        <v>0.1870620156931716</v>
+        <v>0.23286200541450353</v>
       </c>
       <c r="M64" s="4">
         <f t="shared" si="6"/>
-        <v>5.0457617525815013E-2</v>
+        <v>6.4123864164936761E-2</v>
       </c>
     </row>
     <row r="65" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3460,15 +3450,15 @@
       </c>
       <c r="K65" s="12">
         <f t="shared" si="4"/>
-        <v>0.47064407468372338</v>
+        <v>0.55700670113071471</v>
       </c>
       <c r="L65" s="12">
         <f t="shared" si="5"/>
-        <v>0.16882184283889112</v>
+        <v>0.21076111238873818</v>
       </c>
       <c r="M65" s="4">
         <f t="shared" si="6"/>
-        <v>5.0457617525815013E-2</v>
+        <v>6.4123864164936761E-2</v>
       </c>
     </row>
     <row r="66" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3501,15 +3491,15 @@
       </c>
       <c r="K66" s="12">
         <f t="shared" si="4"/>
-        <v>0.48226077020924707</v>
+        <v>0.56941175068304162</v>
       </c>
       <c r="L66" s="12">
         <f t="shared" si="5"/>
-        <v>0.15643492295654537</v>
+        <v>0.19567457386278631</v>
       </c>
       <c r="M66" s="4">
         <f t="shared" si="6"/>
-        <v>4.340834212541933E-2</v>
+        <v>5.5221429161617874E-2</v>
       </c>
     </row>
     <row r="67" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3542,15 +3532,15 @@
       </c>
       <c r="K67" s="12">
         <f t="shared" si="4"/>
-        <v>0.45070081538434603</v>
+        <v>0.53553236001367477</v>
       </c>
       <c r="L67" s="12">
         <f t="shared" si="5"/>
-        <v>0.13750755934931169</v>
+        <v>0.17250232802640764</v>
       </c>
       <c r="M67" s="4">
         <f t="shared" si="6"/>
-        <v>4.340834212541933E-2</v>
+        <v>5.5221429161617874E-2</v>
       </c>
     </row>
     <row r="68" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3583,15 +3573,15 @@
       </c>
       <c r="K68" s="12">
         <f t="shared" si="4"/>
-        <v>0.45876673131239654</v>
+        <v>0.54424426780249591</v>
       </c>
       <c r="L68" s="12">
         <f t="shared" si="5"/>
-        <v>0.1749469262936646</v>
+        <v>0.21819793210070104</v>
       </c>
       <c r="M68" s="4">
         <f t="shared" si="6"/>
-        <v>3.6306733849116646E-2</v>
+        <v>4.6234310570424819E-2</v>
       </c>
     </row>
     <row r="69" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3624,15 +3614,15 @@
       </c>
       <c r="K69" s="12">
         <f t="shared" si="4"/>
-        <v>0.48226077020924707</v>
+        <v>0.56941175068304162</v>
       </c>
       <c r="L69" s="12">
         <f t="shared" si="5"/>
-        <v>0.18102687303857068</v>
+        <v>0.22556467634084354</v>
       </c>
       <c r="M69" s="4">
         <f t="shared" si="6"/>
-        <v>3.6306733849116646E-2</v>
+        <v>4.6234310570424819E-2</v>
       </c>
     </row>
     <row r="70" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3665,15 +3655,15 @@
       </c>
       <c r="K70" s="12">
         <f t="shared" ref="K70:K116" si="72">(1-(1/(2.71828^((C70*($B$1/100))/169))))</f>
-        <v>0.46671420723255974</v>
+        <v>0.55279276843269742</v>
       </c>
       <c r="L70" s="12">
         <f t="shared" ref="L70:L116" si="73">(1-(1/(2.71828^((D70*($B$1/100))/169))))</f>
-        <v>0.1749469262936646</v>
+        <v>0.21819793210070104</v>
       </c>
       <c r="M70" s="4">
         <f t="shared" ref="M70:M116" si="74">IF(E70*($B$1/100)&gt;0, (1-(1/(2.71828^(E70*($B$1/100)/169)))), "&lt;1%")</f>
-        <v>2.9152404184648928E-2</v>
+        <v>3.7161702846576494E-2</v>
       </c>
     </row>
     <row r="71" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3706,15 +3696,15 @@
       </c>
       <c r="K71" s="12">
         <f t="shared" si="72"/>
-        <v>0.47841714354892473</v>
+        <v>0.56531581986916657</v>
       </c>
       <c r="L71" s="12">
         <f t="shared" si="73"/>
-        <v>0.18102687303857068</v>
+        <v>0.22556467634084354</v>
       </c>
       <c r="M71" s="4">
         <f t="shared" si="74"/>
-        <v>3.6306733849116646E-2</v>
+        <v>4.6234310570424819E-2</v>
       </c>
     </row>
     <row r="72" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3747,15 +3737,15 @@
       </c>
       <c r="K72" s="12">
         <f t="shared" si="72"/>
-        <v>0.47064407468372338</v>
+        <v>0.55700670113071471</v>
       </c>
       <c r="L72" s="12">
         <f t="shared" si="73"/>
-        <v>0.1749469262936646</v>
+        <v>0.21819793210070104</v>
       </c>
       <c r="M72" s="4">
         <f t="shared" si="74"/>
-        <v>3.6306733849116646E-2</v>
+        <v>4.6234310570424819E-2</v>
       </c>
     </row>
     <row r="73" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3788,15 +3778,15 @@
       </c>
       <c r="K73" s="12">
         <f t="shared" si="72"/>
-        <v>0.45474868805571345</v>
+        <v>0.5399089336402908</v>
       </c>
       <c r="L73" s="12">
         <f t="shared" si="73"/>
-        <v>0.1870620156931716</v>
+        <v>0.23286200541450353</v>
       </c>
       <c r="M73" s="4">
         <f t="shared" si="74"/>
-        <v>4.340834212541933E-2</v>
+        <v>5.5221429161617874E-2</v>
       </c>
     </row>
     <row r="74" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3829,15 +3819,15 @@
       </c>
       <c r="K74" s="12">
         <f t="shared" si="72"/>
-        <v>0.48607607257608232</v>
+        <v>0.57346908646631989</v>
       </c>
       <c r="L74" s="12">
         <f t="shared" si="73"/>
-        <v>0.20490190865211622</v>
+        <v>0.2543440117125576</v>
       </c>
       <c r="M74" s="4">
         <f t="shared" si="74"/>
-        <v>4.340834212541933E-2</v>
+        <v>5.5221429161617874E-2</v>
       </c>
     </row>
     <row r="75" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3870,15 +3860,15 @@
       </c>
       <c r="K75" s="12">
         <f t="shared" si="72"/>
-        <v>0.50105819062850654</v>
+        <v>0.5893197015299374</v>
       </c>
       <c r="L75" s="12">
         <f t="shared" si="73"/>
-        <v>0.23376932343862444</v>
+        <v>0.28881890225373608</v>
       </c>
       <c r="M75" s="4">
         <f t="shared" si="74"/>
-        <v>5.0457617525815013E-2</v>
+        <v>6.4123864164936761E-2</v>
       </c>
     </row>
     <row r="76" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3911,15 +3901,15 @@
       </c>
       <c r="K76" s="12">
         <f t="shared" si="72"/>
-        <v>0.43420657682699038</v>
+        <v>0.51760576894427923</v>
       </c>
       <c r="L76" s="12">
         <f t="shared" si="73"/>
-        <v>0.1989992069721388</v>
+        <v>0.24725102823281386</v>
       </c>
       <c r="M76" s="4">
         <f t="shared" si="74"/>
-        <v>4.340834212541933E-2</v>
+        <v>5.5221429161617874E-2</v>
       </c>
     </row>
     <row r="77" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3952,15 +3942,15 @@
       </c>
       <c r="K77" s="12">
         <f t="shared" si="72"/>
-        <v>0.46275516497207569</v>
+        <v>0.54853875109044536</v>
       </c>
       <c r="L77" s="12">
         <f t="shared" si="73"/>
-        <v>0.23941579862461304</v>
+        <v>0.29552020104870858</v>
       </c>
       <c r="M77" s="4">
         <f t="shared" si="74"/>
-        <v>4.340834212541933E-2</v>
+        <v>5.5221429161617874E-2</v>
       </c>
     </row>
     <row r="78" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3993,15 +3983,15 @@
       </c>
       <c r="K78" s="12">
         <f t="shared" si="72"/>
-        <v>0.49735411349835601</v>
+        <v>0.585413143253386</v>
       </c>
       <c r="L78" s="12">
         <f t="shared" si="73"/>
-        <v>0.25058422631632693</v>
+        <v>0.30873395916484248</v>
       </c>
       <c r="M78" s="4">
         <f t="shared" si="74"/>
-        <v>5.0457617525815013E-2</v>
+        <v>6.4123864164936761E-2</v>
       </c>
     </row>
     <row r="79" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4034,15 +4024,15 @@
       </c>
       <c r="K79" s="12">
         <f t="shared" si="72"/>
-        <v>0.48226077020924707</v>
+        <v>0.56941175068304162</v>
       </c>
       <c r="L79" s="12">
         <f t="shared" si="73"/>
-        <v>0.25058422631632693</v>
+        <v>0.30873395916484248</v>
       </c>
       <c r="M79" s="4">
         <f t="shared" si="74"/>
-        <v>5.0457617525815013E-2</v>
+        <v>6.4123864164936761E-2</v>
       </c>
     </row>
     <row r="80" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4075,15 +4065,15 @@
       </c>
       <c r="K80" s="12">
         <f t="shared" si="72"/>
-        <v>0.50473497182775517</v>
+        <v>0.59318944919052297</v>
       </c>
       <c r="L80" s="12">
         <f t="shared" si="73"/>
-        <v>0.26703012679379212</v>
+        <v>0.32809133886401298</v>
       </c>
       <c r="M80" s="4">
         <f t="shared" si="74"/>
-        <v>5.0457617525815013E-2</v>
+        <v>6.4123864164936761E-2</v>
       </c>
     </row>
     <row r="81" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4116,15 +4106,15 @@
       </c>
       <c r="K81" s="12">
         <f t="shared" si="72"/>
-        <v>0.50105819062850654</v>
+        <v>0.5893197015299374</v>
       </c>
       <c r="L81" s="12">
         <f t="shared" si="73"/>
-        <v>0.26158865667956688</v>
+        <v>0.32169986999875255</v>
       </c>
       <c r="M81" s="4">
         <f t="shared" si="74"/>
-        <v>4.340834212541933E-2</v>
+        <v>5.5221429161617874E-2</v>
       </c>
     </row>
     <row r="82" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4157,15 +4147,15 @@
       </c>
       <c r="K82" s="12">
         <f t="shared" si="72"/>
-        <v>0.56966646109251018</v>
+        <v>0.66016300909060299</v>
       </c>
       <c r="L82" s="12">
         <f t="shared" si="73"/>
-        <v>0.32928301731501863</v>
+        <v>0.40024992946893767</v>
       </c>
       <c r="M82" s="4">
         <f t="shared" si="74"/>
-        <v>5.0457617525815013E-2</v>
+        <v>6.4123864164936761E-2</v>
       </c>
     </row>
     <row r="83" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4198,15 +4188,15 @@
       </c>
       <c r="K83" s="12">
         <f t="shared" si="72"/>
-        <v>0.58834652657744901</v>
+        <v>0.67892929341060371</v>
       </c>
       <c r="L83" s="12">
         <f t="shared" si="73"/>
-        <v>0.32430370431758404</v>
+        <v>0.39454486250900855</v>
       </c>
       <c r="M83" s="4">
         <f t="shared" si="74"/>
-        <v>4.340834212541933E-2</v>
+        <v>5.5221429161617874E-2</v>
       </c>
     </row>
     <row r="84" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4239,15 +4229,15 @@
       </c>
       <c r="K84" s="12">
         <f t="shared" si="72"/>
-        <v>0.5791101141373356</v>
+        <v>0.66967939392690878</v>
       </c>
       <c r="L84" s="12">
         <f t="shared" si="73"/>
-        <v>0.31928742556772838</v>
+        <v>0.38878552662837995</v>
       </c>
       <c r="M84" s="4">
         <f t="shared" si="74"/>
-        <v>5.0457617525815013E-2</v>
+        <v>6.4123864164936761E-2</v>
       </c>
     </row>
     <row r="85" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4280,15 +4270,15 @@
       </c>
       <c r="K85" s="12">
         <f t="shared" si="72"/>
-        <v>0.44662289184871728</v>
+        <v>0.53111415463606493</v>
       </c>
       <c r="L85" s="12">
         <f t="shared" si="73"/>
-        <v>0.16882184283889112</v>
+        <v>0.21076111238873818</v>
       </c>
       <c r="M85" s="4">
         <f t="shared" si="74"/>
-        <v>2.1944961735495983E-2</v>
+        <v>2.8002792782622188E-2</v>
       </c>
     </row>
     <row r="86" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4321,15 +4311,15 @@
       </c>
       <c r="K86" s="12">
         <f t="shared" si="72"/>
-        <v>0.39077145153385251</v>
+        <v>0.4697035557086614</v>
       </c>
       <c r="L86" s="12">
         <f t="shared" si="73"/>
-        <v>0.14386340271764586</v>
+        <v>0.18029965161896699</v>
       </c>
       <c r="M86" s="4">
         <f t="shared" si="74"/>
-        <v>7.3691583471030553E-3</v>
+        <v>9.4227740532037974E-3</v>
       </c>
     </row>
     <row r="87" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4362,15 +4352,15 @@
       </c>
       <c r="K87" s="12">
         <f t="shared" si="72"/>
-        <v>0.34400187583538788</v>
+        <v>0.41704460641538199</v>
       </c>
       <c r="L87" s="12">
         <f t="shared" si="73"/>
-        <v>0.10501352355029347</v>
+        <v>0.13238892828227111</v>
       </c>
       <c r="M87" s="4">
         <f t="shared" si="74"/>
-        <v>7.3691583471030553E-3</v>
+        <v>9.4227740532037974E-3</v>
       </c>
     </row>
     <row r="88" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4403,15 +4393,15 @@
       </c>
       <c r="K88" s="12">
         <f t="shared" si="72"/>
-        <v>0.33913183367115096</v>
+        <v>0.41149929726334278</v>
       </c>
       <c r="L88" s="12">
         <f t="shared" si="73"/>
-        <v>0.11160882061376709</v>
+        <v>0.14056423137712515</v>
       </c>
       <c r="M88" s="4">
         <f t="shared" si="74"/>
-        <v>7.3691583471030553E-3</v>
+        <v>9.4227740532037974E-3</v>
       </c>
     </row>
     <row r="89" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4444,15 +4434,15 @@
       </c>
       <c r="K89" s="12">
         <f t="shared" si="72"/>
-        <v>0.30401404031397616</v>
+        <v>0.37117671858194146</v>
       </c>
       <c r="L89" s="12">
         <f t="shared" si="73"/>
-        <v>9.8369263885248692E-2</v>
+        <v>0.12413585837442997</v>
       </c>
       <c r="M89" s="4">
         <f t="shared" si="74"/>
-        <v>1.4684012199461582E-2</v>
+        <v>1.8756759435549886E-2</v>
       </c>
     </row>
     <row r="90" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4485,11 +4475,11 @@
       </c>
       <c r="K90" s="12">
         <f t="shared" si="72"/>
-        <v>0.23941579862461304</v>
+        <v>0.29552020104870858</v>
       </c>
       <c r="L90" s="12">
         <f t="shared" si="73"/>
-        <v>5.7454945699552895E-2</v>
+        <v>7.2942413534695993E-2</v>
       </c>
       <c r="M90" s="4" t="str">
         <f t="shared" si="74"/>
@@ -4526,15 +4516,15 @@
       </c>
       <c r="K91" s="12">
         <f t="shared" si="72"/>
-        <v>0.22235030584271132</v>
+        <v>0.27522446183969218</v>
       </c>
       <c r="L91" s="12">
         <f t="shared" si="73"/>
-        <v>7.8139060850156983E-2</v>
+        <v>9.8902615026041585E-2</v>
       </c>
       <c r="M91" s="4">
         <f t="shared" si="74"/>
-        <v>7.3691583471030553E-3</v>
+        <v>9.4227740532037974E-3</v>
       </c>
     </row>
     <row r="92" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4567,15 +4557,15 @@
       </c>
       <c r="K92" s="12">
         <f t="shared" si="72"/>
-        <v>0.22235030584271132</v>
+        <v>0.27522446183969218</v>
       </c>
       <c r="L92" s="12">
         <f t="shared" si="73"/>
-        <v>7.8139060850156983E-2</v>
+        <v>9.8902615026041585E-2</v>
       </c>
       <c r="M92" s="4">
         <f t="shared" si="74"/>
-        <v>7.3691583471030553E-3</v>
+        <v>9.4227740532037974E-3</v>
       </c>
     </row>
     <row r="93" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4608,15 +4598,15 @@
       </c>
       <c r="K93" s="12">
         <f t="shared" si="72"/>
-        <v>0.21657713872523698</v>
+        <v>0.26833010170654215</v>
       </c>
       <c r="L93" s="12">
         <f t="shared" si="73"/>
-        <v>7.8139060850156983E-2</v>
+        <v>9.8902615026041585E-2</v>
       </c>
       <c r="M93" s="4">
         <f t="shared" si="74"/>
-        <v>7.3691583471030553E-3</v>
+        <v>9.4227740532037974E-3</v>
       </c>
     </row>
     <row r="94" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4649,11 +4639,11 @@
       </c>
       <c r="K94" s="12">
         <f t="shared" si="72"/>
-        <v>0.18102687303857068</v>
+        <v>0.22556467634084354</v>
       </c>
       <c r="L94" s="12">
         <f t="shared" si="73"/>
-        <v>4.340834212541933E-2</v>
+        <v>5.5221429161617874E-2</v>
       </c>
       <c r="M94" s="4" t="str">
         <f t="shared" si="74"/>
@@ -4690,11 +4680,11 @@
       </c>
       <c r="K95" s="12">
         <f t="shared" si="72"/>
-        <v>0.16265128758536473</v>
+        <v>0.20325355061852413</v>
       </c>
       <c r="L95" s="12">
         <f t="shared" si="73"/>
-        <v>4.340834212541933E-2</v>
+        <v>5.5221429161617874E-2</v>
       </c>
       <c r="M95" s="4" t="str">
         <f t="shared" si="74"/>
@@ -4731,15 +4721,15 @@
       </c>
       <c r="K96" s="12">
         <f t="shared" si="72"/>
-        <v>0.1749469262936646</v>
+        <v>0.21819793210070104</v>
       </c>
       <c r="L96" s="12">
         <f t="shared" si="73"/>
-        <v>5.0457617525815013E-2</v>
+        <v>6.4123864164936761E-2</v>
       </c>
       <c r="M96" s="4">
         <f t="shared" si="74"/>
-        <v>7.3691583471030553E-3</v>
+        <v>9.4227740532037974E-3</v>
       </c>
     </row>
     <row r="97" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4772,15 +4762,15 @@
       </c>
       <c r="K97" s="12">
         <f t="shared" si="72"/>
-        <v>0.1870620156931716</v>
+        <v>0.23286200541450353</v>
       </c>
       <c r="L97" s="12">
         <f t="shared" si="73"/>
-        <v>5.7454945699552895E-2</v>
+        <v>7.2942413534695993E-2</v>
       </c>
       <c r="M97" s="4">
         <f t="shared" si="74"/>
-        <v>1.4684012199461582E-2</v>
+        <v>1.8756759435549886E-2</v>
       </c>
     </row>
     <row r="98" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4813,15 +4803,15 @@
       </c>
       <c r="K98" s="12">
         <f t="shared" si="72"/>
-        <v>0.26158865667956688</v>
+        <v>0.32169986999875255</v>
       </c>
       <c r="L98" s="12">
         <f t="shared" si="73"/>
-        <v>9.8369263885248692E-2</v>
+        <v>0.12413585837442997</v>
       </c>
       <c r="M98" s="4">
         <f t="shared" si="74"/>
-        <v>2.9152404184648928E-2</v>
+        <v>3.7161702846576494E-2</v>
       </c>
     </row>
     <row r="99" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4854,15 +4844,15 @@
       </c>
       <c r="K99" s="12">
         <f t="shared" si="72"/>
-        <v>0.24502066404085332</v>
+        <v>0.30215835501927313</v>
       </c>
       <c r="L99" s="12">
         <f t="shared" si="73"/>
-        <v>9.1675678126840299E-2</v>
+        <v>0.11580428190400116</v>
       </c>
       <c r="M99" s="4">
         <f t="shared" si="74"/>
-        <v>2.9152404184648928E-2</v>
+        <v>3.7161702846576494E-2</v>
       </c>
     </row>
     <row r="100" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4895,15 +4885,15 @@
       </c>
       <c r="K100" s="12">
         <f t="shared" si="72"/>
-        <v>0.21076111238873818</v>
+        <v>0.26137015961160848</v>
       </c>
       <c r="L100" s="12">
         <f t="shared" si="73"/>
-        <v>9.8369263885248692E-2</v>
+        <v>0.12413585837442997</v>
       </c>
       <c r="M100" s="4">
         <f t="shared" si="74"/>
-        <v>2.9152404184648928E-2</v>
+        <v>3.7161702846576494E-2</v>
       </c>
     </row>
     <row r="101" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4936,15 +4926,15 @@
       </c>
       <c r="K101" s="12">
         <f t="shared" si="72"/>
-        <v>0.23376932343862444</v>
+        <v>0.28881890225373608</v>
       </c>
       <c r="L101" s="12">
         <f t="shared" si="73"/>
-        <v>0.10501352355029347</v>
+        <v>0.13238892828227111</v>
       </c>
       <c r="M101" s="4">
         <f t="shared" si="74"/>
-        <v>2.9152404184648928E-2</v>
+        <v>3.7161702846576494E-2</v>
       </c>
     </row>
     <row r="102" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4977,15 +4967,15 @@
       </c>
       <c r="K102" s="12">
         <f t="shared" si="72"/>
-        <v>0.26158865667956688</v>
+        <v>0.32169986999875255</v>
       </c>
       <c r="L102" s="12">
         <f t="shared" si="73"/>
-        <v>0.10501352355029347</v>
+        <v>0.13238892828227111</v>
       </c>
       <c r="M102" s="4">
         <f t="shared" si="74"/>
-        <v>2.9152404184648928E-2</v>
+        <v>3.7161702846576494E-2</v>
       </c>
     </row>
     <row r="103" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5018,15 +5008,15 @@
       </c>
       <c r="K103" s="12">
         <f t="shared" si="72"/>
-        <v>0.21657713872523698</v>
+        <v>0.26833010170654215</v>
       </c>
       <c r="L103" s="12">
         <f t="shared" si="73"/>
-        <v>8.4932400084761439E-2</v>
+        <v>0.10739345208458406</v>
       </c>
       <c r="M103" s="4">
         <f t="shared" si="74"/>
-        <v>1.4684012199461582E-2</v>
+        <v>1.8756759435549886E-2</v>
       </c>
     </row>
     <row r="104" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5059,15 +5049,15 @@
       </c>
       <c r="K104" s="12">
         <f t="shared" si="72"/>
-        <v>0.24502066404085332</v>
+        <v>0.30215835501927313</v>
       </c>
       <c r="L104" s="12">
         <f t="shared" si="73"/>
-        <v>0.11815551588883388</v>
+        <v>0.14866250043810003</v>
       </c>
       <c r="M104" s="4">
         <f t="shared" si="74"/>
-        <v>2.1944961735495983E-2</v>
+        <v>2.8002792782622188E-2</v>
       </c>
     </row>
     <row r="105" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5100,15 +5090,15 @@
       </c>
       <c r="K105" s="12">
         <f t="shared" si="72"/>
-        <v>0.22808092957753268</v>
+        <v>0.28205385797506577</v>
       </c>
       <c r="L105" s="12">
         <f t="shared" si="73"/>
-        <v>0.11160882061376709</v>
+        <v>0.14056423137712515</v>
       </c>
       <c r="M105" s="4">
         <f t="shared" si="74"/>
-        <v>2.9152404184648928E-2</v>
+        <v>3.7161702846576494E-2</v>
       </c>
     </row>
     <row r="106" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5141,15 +5131,15 @@
       </c>
       <c r="K106" s="12">
         <f t="shared" si="72"/>
-        <v>0.22235030584271132</v>
+        <v>0.27522446183969218</v>
       </c>
       <c r="L106" s="12">
         <f t="shared" si="73"/>
-        <v>0.10501352355029347</v>
+        <v>0.13238892828227111</v>
       </c>
       <c r="M106" s="4">
         <f t="shared" si="74"/>
-        <v>2.9152404184648928E-2</v>
+        <v>3.7161702846576494E-2</v>
       </c>
     </row>
     <row r="107" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5182,15 +5172,15 @@
       </c>
       <c r="K107" s="12">
         <f t="shared" si="72"/>
-        <v>0.1989992069721388</v>
+        <v>0.24725102823281386</v>
       </c>
       <c r="L107" s="12">
         <f t="shared" si="73"/>
-        <v>7.8139060850156983E-2</v>
+        <v>9.8902615026041585E-2</v>
       </c>
       <c r="M107" s="4">
         <f t="shared" si="74"/>
-        <v>1.4684012199461582E-2</v>
+        <v>1.8756759435549886E-2</v>
       </c>
     </row>
     <row r="108" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5223,15 +5213,15 @@
       </c>
       <c r="K108" s="12">
         <f t="shared" si="72"/>
-        <v>0.1989992069721388</v>
+        <v>0.24725102823281386</v>
       </c>
       <c r="L108" s="12">
         <f t="shared" si="73"/>
-        <v>7.1295288775442778E-2</v>
+        <v>9.0331009666926976E-2</v>
       </c>
       <c r="M108" s="4">
         <f t="shared" si="74"/>
-        <v>1.4684012199461582E-2</v>
+        <v>1.8756759435549886E-2</v>
       </c>
     </row>
     <row r="109" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5264,15 +5254,15 @@
       </c>
       <c r="K109" s="12">
         <f t="shared" si="72"/>
-        <v>0.1870620156931716</v>
+        <v>0.23286200541450353</v>
       </c>
       <c r="L109" s="12">
         <f t="shared" si="73"/>
-        <v>5.7454945699552895E-2</v>
+        <v>7.2942413534695993E-2</v>
       </c>
       <c r="M109" s="4">
         <f t="shared" si="74"/>
-        <v>1.4684012199461582E-2</v>
+        <v>1.8756759435549886E-2</v>
       </c>
     </row>
     <row r="110" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5305,15 +5295,15 @@
       </c>
       <c r="K110" s="12">
         <f t="shared" si="72"/>
-        <v>0.1870620156931716</v>
+        <v>0.23286200541450353</v>
       </c>
       <c r="L110" s="12">
         <f t="shared" si="73"/>
-        <v>5.7454945699552895E-2</v>
+        <v>7.2942413534695993E-2</v>
       </c>
       <c r="M110" s="4">
         <f t="shared" si="74"/>
-        <v>1.4684012199461582E-2</v>
+        <v>1.8756759435549886E-2</v>
       </c>
     </row>
     <row r="111" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5346,11 +5336,11 @@
       </c>
       <c r="K111" s="12">
         <f t="shared" si="72"/>
-        <v>0.16265128758536473</v>
+        <v>0.20325355061852413</v>
       </c>
       <c r="L111" s="12">
         <f t="shared" si="73"/>
-        <v>4.340834212541933E-2</v>
+        <v>5.5221429161617874E-2</v>
       </c>
       <c r="M111" s="4" t="str">
         <f t="shared" si="74"/>
@@ -5387,11 +5377,11 @@
       </c>
       <c r="K112" s="12">
         <f t="shared" si="72"/>
-        <v>0.15643492295654537</v>
+        <v>0.19567457386278631</v>
       </c>
       <c r="L112" s="12">
         <f t="shared" si="73"/>
-        <v>4.340834212541933E-2</v>
+        <v>5.5221429161617874E-2</v>
       </c>
       <c r="M112" s="4" t="str">
         <f t="shared" si="74"/>
@@ -5428,11 +5418,11 @@
       </c>
       <c r="K113" s="12">
         <f t="shared" si="72"/>
-        <v>0.15017240886976957</v>
+        <v>0.18802350279309388</v>
       </c>
       <c r="L113" s="12">
         <f t="shared" si="73"/>
-        <v>4.340834212541933E-2</v>
+        <v>5.5221429161617874E-2</v>
       </c>
       <c r="M113" s="4" t="str">
         <f t="shared" si="74"/>
@@ -5469,15 +5459,15 @@
       </c>
       <c r="K114" s="12">
         <f t="shared" si="72"/>
-        <v>0.1749469262936646</v>
+        <v>0.21819793210070104</v>
       </c>
       <c r="L114" s="12">
         <f t="shared" si="73"/>
-        <v>5.7454945699552895E-2</v>
+        <v>7.2942413534695993E-2</v>
       </c>
       <c r="M114" s="4">
         <f t="shared" si="74"/>
-        <v>7.3691583471030553E-3</v>
+        <v>9.4227740532037974E-3</v>
       </c>
     </row>
     <row r="115" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5510,15 +5500,15 @@
       </c>
       <c r="K115" s="12">
         <f t="shared" si="72"/>
-        <v>0.15017240886976957</v>
+        <v>0.18802350279309388</v>
       </c>
       <c r="L115" s="12">
         <f t="shared" si="73"/>
-        <v>5.7454945699552895E-2</v>
+        <v>7.2942413534695993E-2</v>
       </c>
       <c r="M115" s="4">
         <f t="shared" si="74"/>
-        <v>7.3691583471030553E-3</v>
+        <v>9.4227740532037974E-3</v>
       </c>
     </row>
     <row r="116" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5551,15 +5541,15 @@
       </c>
       <c r="K116" s="12">
         <f t="shared" si="72"/>
-        <v>0.16265128758536473</v>
+        <v>0.20325355061852413</v>
       </c>
       <c r="L116" s="12">
         <f t="shared" si="73"/>
-        <v>5.0457617525815013E-2</v>
+        <v>6.4123864164936761E-2</v>
       </c>
       <c r="M116" s="4">
         <f t="shared" si="74"/>
-        <v>7.3691583471030553E-3</v>
+        <v>9.4227740532037974E-3</v>
       </c>
     </row>
     <row r="117" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8240,21 +8230,21 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="30.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="30.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.25" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="7.625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="18.625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="18.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.1640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.1640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="7.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="26" width="7.625" style="1" customWidth="1"/>
-    <col min="27" max="16384" width="12.625" style="1"/>
+    <col min="13" max="26" width="7.6640625" style="1" customWidth="1"/>
+    <col min="27" max="16384" width="12.6640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -8263,10 +8253,10 @@
       </c>
       <c r="B1" s="1">
         <f>County!B1</f>
-        <v>125</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F2" s="2"/>
       <c r="G2" s="11" t="s">
         <v>180</v>
@@ -8278,7 +8268,7 @@
       </c>
       <c r="L2" s="4"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
         <v>128</v>
       </c>
@@ -8299,7 +8289,7 @@
       <c r="K3" s="2"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
@@ -8331,7 +8321,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>6</v>
       </c>
@@ -8358,18 +8348,18 @@
       </c>
       <c r="J5" s="12">
         <f>(1-(1/(2.71828^((B5*($B$1/100))/169))))</f>
-        <v>0.65784262457167453</v>
+        <v>0.74659851268682298</v>
       </c>
       <c r="K5" s="12">
         <f t="shared" ref="K5:K20" si="1">(1-(1/(2.71828^((C5*($B$1/100))/169))))</f>
-        <v>0.41289055029629673</v>
+        <v>0.49422144620841901</v>
       </c>
       <c r="L5" s="4">
         <f>IF(D5*($B$1/100)&gt;0, (1-(1/(2.71828^(D5*($B$1/100)/169)))), "&lt;1%")</f>
-        <v>0.16882184283889112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.21076111238873818</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>20</v>
       </c>
@@ -8396,18 +8386,18 @@
       </c>
       <c r="J6" s="12">
         <f t="shared" ref="J6:J20" si="3">(1-(1/(2.71828^((B6*($B$1/100))/169))))</f>
-        <v>0.71560626323240273</v>
+        <v>0.80000569203390892</v>
       </c>
       <c r="K6" s="12">
         <f t="shared" si="1"/>
-        <v>0.44251469435523794</v>
+        <v>0.52665392148928847</v>
       </c>
       <c r="L6" s="4">
         <f t="shared" ref="L6:L20" si="4">IF(D6*($B$1/100)&gt;0, (1-(1/(2.71828^(D6*($B$1/100)/169)))), "&lt;1%")</f>
-        <v>0.18102687303857068</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.22556467634084354</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>29</v>
       </c>
@@ -8434,18 +8424,18 @@
       </c>
       <c r="J7" s="12">
         <f t="shared" si="3"/>
-        <v>0.59738024629999087</v>
+        <v>0.68792016987579663</v>
       </c>
       <c r="K7" s="12">
         <f t="shared" si="1"/>
-        <v>0.31928742556772838</v>
+        <v>0.38878552662837995</v>
       </c>
       <c r="L7" s="4">
         <f t="shared" si="4"/>
-        <v>9.8369263885248692E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.12413585837442997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>33</v>
       </c>
@@ -8472,18 +8462,18 @@
       </c>
       <c r="J8" s="12">
         <f t="shared" si="3"/>
-        <v>0.65784262457167453</v>
+        <v>0.74659851268682298</v>
       </c>
       <c r="K8" s="12">
         <f t="shared" si="1"/>
-        <v>0.33913183367115096</v>
+        <v>0.41149929726334278</v>
       </c>
       <c r="L8" s="4">
         <f t="shared" si="4"/>
-        <v>0.11160882061376709</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.14056423137712515</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>36</v>
       </c>
@@ -8510,18 +8500,18 @@
       </c>
       <c r="J9" s="12">
         <f t="shared" si="3"/>
-        <v>0.91607309052217223</v>
+        <v>0.95806336539243997</v>
       </c>
       <c r="K9" s="12">
         <f t="shared" si="1"/>
-        <v>0.66286686764659974</v>
+        <v>0.75135150342496682</v>
       </c>
       <c r="L9" s="4">
         <f t="shared" si="4"/>
-        <v>0.33422563696651553</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.40590123887194485</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>70</v>
       </c>
@@ -8548,18 +8538,18 @@
       </c>
       <c r="J10" s="12">
         <f t="shared" si="3"/>
-        <v>0.70706654886573239</v>
+        <v>0.79228671256911687</v>
       </c>
       <c r="K10" s="12">
         <f t="shared" si="1"/>
-        <v>0.37247766684275874</v>
+        <v>0.44923623638659793</v>
       </c>
       <c r="L10" s="4">
         <f t="shared" si="4"/>
-        <v>8.4932400084761439E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.10739345208458406</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>77</v>
       </c>
@@ -8586,18 +8576,18 @@
       </c>
       <c r="J11" s="12">
         <f t="shared" si="3"/>
-        <v>0.64495199100545064</v>
+        <v>0.73431473775835832</v>
       </c>
       <c r="K11" s="12">
         <f t="shared" si="1"/>
-        <v>0.33913183367115096</v>
+        <v>0.41149929726334278</v>
       </c>
       <c r="L11" s="4">
         <f t="shared" si="4"/>
-        <v>9.1675678126840299E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.11580428190400116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>84</v>
       </c>
@@ -8624,18 +8614,18 @@
       </c>
       <c r="J12" s="12">
         <f t="shared" si="3"/>
-        <v>0.76361813796534705</v>
+        <v>0.84215671485225818</v>
       </c>
       <c r="K12" s="12">
         <f t="shared" si="1"/>
-        <v>0.43837599815410178</v>
+        <v>0.52215126078808638</v>
       </c>
       <c r="L12" s="4">
         <f t="shared" si="4"/>
-        <v>8.4932400084761439E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.10739345208458406</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>93</v>
       </c>
@@ -8662,18 +8652,18 @@
       </c>
       <c r="J13" s="12">
         <f t="shared" si="3"/>
-        <v>0.54004503503167323</v>
+        <v>0.62993705698830182</v>
       </c>
       <c r="K13" s="12">
         <f t="shared" si="1"/>
-        <v>0.22808092957753268</v>
+        <v>0.28205385797506577</v>
       </c>
       <c r="L13" s="4">
         <f t="shared" si="4"/>
-        <v>2.1944961735495983E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+        <v>2.8002792782622188E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>97</v>
       </c>
@@ -8700,18 +8690,18 @@
       </c>
       <c r="J14" s="12">
         <f t="shared" si="3"/>
-        <v>0.39526095317707544</v>
+        <v>0.47470041928443607</v>
       </c>
       <c r="K14" s="12">
         <f t="shared" si="1"/>
-        <v>0.13110453105155007</v>
+        <v>0.16463083311584525</v>
       </c>
       <c r="L14" s="4">
         <f t="shared" si="4"/>
-        <v>1.4684012199461582E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1.8756759435549886E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>99</v>
       </c>
@@ -8737,18 +8727,18 @@
       </c>
       <c r="J15" s="12">
         <f t="shared" si="3"/>
-        <v>0.26703012679379212</v>
+        <v>0.32809133886401298</v>
       </c>
       <c r="K15" s="12">
         <f t="shared" si="1"/>
-        <v>6.4400709453971694E-2</v>
+        <v>8.1677867706266838E-2</v>
       </c>
       <c r="L15" s="4" t="str">
         <f t="shared" si="4"/>
         <v>&lt;1%</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>101</v>
       </c>
@@ -8775,18 +8765,18 @@
       </c>
       <c r="J16" s="12">
         <f t="shared" si="3"/>
-        <v>0.27779306535378978</v>
+        <v>0.34069416798360319</v>
       </c>
       <c r="K16" s="12">
         <f t="shared" si="1"/>
-        <v>8.4932400084761439E-2</v>
+        <v>0.10739345208458406</v>
       </c>
       <c r="L16" s="4">
         <f t="shared" si="4"/>
-        <v>7.3691583471030553E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+        <v>9.4227740532037974E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>106</v>
       </c>
@@ -8813,18 +8803,18 @@
       </c>
       <c r="J17" s="12">
         <f t="shared" si="3"/>
-        <v>0.32928301731501863</v>
+        <v>0.40024992946893767</v>
       </c>
       <c r="K17" s="12">
         <f t="shared" si="1"/>
-        <v>0.11815551588883388</v>
+        <v>0.14866250043810003</v>
       </c>
       <c r="L17" s="4">
         <f t="shared" si="4"/>
-        <v>2.9152404184648928E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+        <v>3.7161702846576494E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>133</v>
       </c>
@@ -8851,18 +8841,18 @@
       </c>
       <c r="J18" s="12">
         <f t="shared" si="3"/>
-        <v>0.27243149785310483</v>
+        <v>0.33442258236228806</v>
       </c>
       <c r="K18" s="12">
         <f t="shared" si="1"/>
-        <v>0.10501352355029347</v>
+        <v>0.13238892828227111</v>
       </c>
       <c r="L18" s="4">
         <f t="shared" si="4"/>
-        <v>2.1944961735495983E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+        <v>2.8002792782622188E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>110</v>
       </c>
@@ -8889,18 +8879,18 @@
       </c>
       <c r="J19" s="12">
         <f t="shared" si="3"/>
-        <v>0.26703012679379212</v>
+        <v>0.32809133886401298</v>
       </c>
       <c r="K19" s="12">
         <f t="shared" si="1"/>
-        <v>0.10501352355029347</v>
+        <v>0.13238892828227111</v>
       </c>
       <c r="L19" s="4">
         <f t="shared" si="4"/>
-        <v>2.9152404184648928E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+        <v>3.7161702846576494E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>114</v>
       </c>
@@ -8927,18 +8917,18 @@
       </c>
       <c r="J20" s="12">
         <f t="shared" si="3"/>
-        <v>0.40853192841956476</v>
+        <v>0.48941027459201225</v>
       </c>
       <c r="K20" s="12">
         <f t="shared" si="1"/>
-        <v>0.1870620156931716</v>
+        <v>0.23286200541450353</v>
       </c>
       <c r="L20" s="4">
         <f t="shared" si="4"/>
-        <v>4.340834212541933E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+        <v>5.5221429161617874E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>120</v>
       </c>
@@ -8965,18 +8955,18 @@
       </c>
       <c r="J21" s="12">
         <f t="shared" ref="J21:J22" si="20">(1-(1/(2.71828^((B21*($B$1/100))/169))))</f>
-        <v>0.22235030584271132</v>
+        <v>0.27522446183969218</v>
       </c>
       <c r="K21" s="12">
         <f t="shared" ref="K21:K22" si="21">(1-(1/(2.71828^((C21*($B$1/100))/169))))</f>
-        <v>7.8139060850156983E-2</v>
+        <v>9.8902615026041585E-2</v>
       </c>
       <c r="L21" s="4">
         <f t="shared" ref="L21:L22" si="22">IF(D21*($B$1/100)&gt;0, (1-(1/(2.71828^(D21*($B$1/100)/169)))), "&lt;1%")</f>
-        <v>2.1944961735495983E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+        <v>2.8002792782622188E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>122</v>
       </c>
@@ -9003,15 +8993,15 @@
       </c>
       <c r="J22" s="12">
         <f t="shared" si="20"/>
-        <v>0.27779306535378978</v>
+        <v>0.34069416798360319</v>
       </c>
       <c r="K22" s="12">
         <f t="shared" si="21"/>
-        <v>9.8369263885248692E-2</v>
+        <v>0.12413585837442997</v>
       </c>
       <c r="L22" s="4">
         <f t="shared" si="22"/>
-        <v>2.1944961735495983E-2</v>
+        <v>2.8002792782622188E-2</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10008,21 +9998,21 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="30.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="30.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="27.125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="27.1640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.5" style="1" customWidth="1"/>
-    <col min="10" max="10" width="41.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="41.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="23" width="7.625" style="1" customWidth="1"/>
-    <col min="24" max="16384" width="12.625" style="1"/>
+    <col min="13" max="23" width="7.6640625" style="1" customWidth="1"/>
+    <col min="24" max="16384" width="12.6640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -10031,10 +10021,10 @@
       </c>
       <c r="B1" s="1">
         <f>County!B1</f>
-        <v>125</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F2" s="2"/>
       <c r="G2" s="11" t="s">
         <v>180</v>
@@ -10046,7 +10036,7 @@
       </c>
       <c r="L2" s="4"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
         <v>128</v>
       </c>
@@ -10067,7 +10057,7 @@
       <c r="K3" s="2"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>134</v>
       </c>
@@ -10099,7 +10089,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>135</v>
       </c>
@@ -10126,18 +10116,18 @@
       </c>
       <c r="J5" s="12">
         <f>(1-(1/(2.71828^((B5*($B$1/100))/169))))</f>
-        <v>0.23376932343862444</v>
+        <v>0.28881890225373608</v>
       </c>
       <c r="K5" s="12">
         <f t="shared" ref="K5:K8" si="1">(1-(1/(2.71828^((C5*($B$1/100))/169))))</f>
-        <v>9.1675678126840299E-2</v>
+        <v>0.11580428190400116</v>
       </c>
       <c r="L5" s="4">
         <f>IF(D5*($B$1/100)&gt;0, (1-(1/(2.71828^(D5*($B$1/100)/169)))), "&lt;1%")</f>
-        <v>7.3691583471030553E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+        <v>9.4227740532037974E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>136</v>
       </c>
@@ -10164,18 +10154,18 @@
       </c>
       <c r="J6" s="12">
         <f t="shared" ref="J6:J8" si="2">(1-(1/(2.71828^((B6*($B$1/100))/169))))</f>
-        <v>0.52271642739038016</v>
+        <v>0.61199805453997391</v>
       </c>
       <c r="K6" s="12">
         <f t="shared" si="1"/>
-        <v>0.34883602988775952</v>
+        <v>0.42253766337222631</v>
       </c>
       <c r="L6" s="4">
         <f t="shared" ref="L6:L8" si="3">IF(D6*($B$1/100)&gt;0, (1-(1/(2.71828^(D6*($B$1/100)/169)))), "&lt;1%")</f>
-        <v>1.4684012199461582E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1.8756759435549886E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>137</v>
       </c>
@@ -10201,18 +10191,18 @@
       </c>
       <c r="J7" s="12">
         <f t="shared" si="2"/>
-        <v>0.15017240886976957</v>
+        <v>0.18802350279309388</v>
       </c>
       <c r="K7" s="12">
         <f t="shared" si="1"/>
-        <v>7.8139060850156983E-2</v>
+        <v>9.8902615026041585E-2</v>
       </c>
       <c r="L7" s="4" t="str">
         <f t="shared" si="3"/>
         <v>&lt;1%</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>138</v>
       </c>
@@ -10239,15 +10229,15 @@
       </c>
       <c r="J8" s="12">
         <f t="shared" si="2"/>
-        <v>0.32430370431758404</v>
+        <v>0.39454486250900855</v>
       </c>
       <c r="K8" s="12">
         <f t="shared" si="1"/>
-        <v>0.1989992069721388</v>
+        <v>0.24725102823281386</v>
       </c>
       <c r="L8" s="4">
         <f t="shared" si="3"/>
-        <v>7.3691583471030553E-3</v>
+        <v>9.4227740532037974E-3</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -11237,21 +11227,21 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.75" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="30.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="30.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.25" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="7.625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="16.375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="18.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.1640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.1640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="7.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="26" width="7.625" style="1" customWidth="1"/>
-    <col min="27" max="16384" width="12.625" style="1"/>
+    <col min="13" max="26" width="7.6640625" style="1" customWidth="1"/>
+    <col min="27" max="16384" width="12.6640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
@@ -11260,10 +11250,10 @@
       </c>
       <c r="B1" s="1">
         <f>County!B1</f>
-        <v>125</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F2" s="2"/>
       <c r="G2" s="11" t="s">
         <v>180</v>
@@ -11275,7 +11265,7 @@
       </c>
       <c r="L2" s="4"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
         <v>128</v>
       </c>
@@ -11355,15 +11345,15 @@
       </c>
       <c r="J5" s="12">
         <f>(1-(1/(2.71828^((B5*($B$1/100))/169))))</f>
-        <v>0.44251469435523794</v>
+        <v>0.52665392148928847</v>
       </c>
       <c r="K5" s="12">
         <f t="shared" ref="K5:K8" si="1">(1-(1/(2.71828^((C5*($B$1/100))/169))))</f>
-        <v>0.22808092957753268</v>
+        <v>0.28205385797506577</v>
       </c>
       <c r="L5" s="4">
         <f>IF(D5*($B$1/100)&gt;0, (1-(1/(2.71828^(D5*($B$1/100)/169)))), "&lt;1%")</f>
-        <v>0.11160882061376709</v>
+        <v>0.14056423137712515</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -11393,15 +11383,15 @@
       </c>
       <c r="J6" s="12">
         <f t="shared" ref="J6:J8" si="3">(1-(1/(2.71828^((B6*($B$1/100))/169))))</f>
-        <v>0.49362253779597032</v>
+        <v>0.58146942420329639</v>
       </c>
       <c r="K6" s="12">
         <f t="shared" si="1"/>
-        <v>0.27779306535378978</v>
+        <v>0.34069416798360319</v>
       </c>
       <c r="L6" s="4">
         <f t="shared" ref="L6:L8" si="4">IF(D6*($B$1/100)&gt;0, (1-(1/(2.71828^(D6*($B$1/100)/169)))), "&lt;1%")</f>
-        <v>0.11160882061376709</v>
+        <v>0.14056423137712515</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -11431,11 +11421,11 @@
       </c>
       <c r="J7" s="12">
         <f t="shared" si="3"/>
-        <v>0.11815551588883388</v>
+        <v>0.14866250043810003</v>
       </c>
       <c r="K7" s="12">
         <f t="shared" si="1"/>
-        <v>5.7454945699552895E-2</v>
+        <v>7.2942413534695993E-2</v>
       </c>
       <c r="L7" s="4" t="str">
         <f t="shared" si="4"/>
@@ -11469,15 +11459,15 @@
       </c>
       <c r="J8" s="12">
         <f t="shared" si="3"/>
-        <v>0.88292833043999996</v>
+        <v>0.93578768622746977</v>
       </c>
       <c r="K8" s="12">
         <f t="shared" si="1"/>
-        <v>0.61485730231505298</v>
+        <v>0.70515366410777003</v>
       </c>
       <c r="L8" s="4">
         <f t="shared" si="4"/>
-        <v>0.32928301731501863</v>
+        <v>0.40024992946893767</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -11507,15 +11497,15 @@
       </c>
       <c r="J9" s="12">
         <f>(1-(1/(2.71828^((B9*($B$1/100))/169))))</f>
-        <v>0.41289055029629673</v>
+        <v>0.49422144620841901</v>
       </c>
       <c r="K9" s="12">
         <f t="shared" ref="K9:K12" si="5">(1-(1/(2.71828^((C9*($B$1/100))/169))))</f>
-        <v>9.8369263885248692E-2</v>
+        <v>0.12413585837442997</v>
       </c>
       <c r="L9" s="4">
         <f>IF(D9*($B$1/100)&gt;0, (1-(1/(2.71828^(D9*($B$1/100)/169)))), "&lt;1%")</f>
-        <v>1.4684012199461582E-2</v>
+        <v>1.8756759435549886E-2</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -11545,15 +11535,15 @@
       </c>
       <c r="J10" s="12">
         <f t="shared" ref="J10:J12" si="6">(1-(1/(2.71828^((B10*($B$1/100))/169))))</f>
-        <v>0.46671420723255974</v>
+        <v>0.55279276843269742</v>
       </c>
       <c r="K10" s="12">
         <f t="shared" si="5"/>
-        <v>0.21657713872523698</v>
+        <v>0.26833010170654215</v>
       </c>
       <c r="L10" s="4">
         <f t="shared" ref="L10:L12" si="7">IF(D10*($B$1/100)&gt;0, (1-(1/(2.71828^(D10*($B$1/100)/169)))), "&lt;1%")</f>
-        <v>6.4400709453971694E-2</v>
+        <v>8.1677867706266838E-2</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -11583,15 +11573,15 @@
       </c>
       <c r="J11" s="12">
         <f t="shared" si="6"/>
-        <v>0.47841714354892473</v>
+        <v>0.56531581986916657</v>
       </c>
       <c r="K11" s="12">
         <f t="shared" si="5"/>
-        <v>0.31423390663665962</v>
+        <v>0.38297140559897314</v>
       </c>
       <c r="L11" s="4">
         <f t="shared" si="7"/>
-        <v>0.12465396752976854</v>
+        <v>0.15668446133949132</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -11621,11 +11611,11 @@
       </c>
       <c r="J12" s="12">
         <f t="shared" si="6"/>
-        <v>0.10501352355029347</v>
+        <v>0.13238892828227111</v>
       </c>
       <c r="K12" s="12">
         <f t="shared" si="5"/>
-        <v>5.0457617525815013E-2</v>
+        <v>6.4123864164936761E-2</v>
       </c>
       <c r="L12" s="4" t="str">
         <f t="shared" si="7"/>
@@ -11659,11 +11649,11 @@
       </c>
       <c r="J13" s="12">
         <f t="shared" ref="J13:J42" si="8">(1-(1/(2.71828^((B13*($B$1/100))/169))))</f>
-        <v>0.1930526844259034</v>
+        <v>0.24009057340511064</v>
       </c>
       <c r="K13" s="12">
         <f t="shared" ref="K13:K42" si="9">(1-(1/(2.71828^((C13*($B$1/100))/169))))</f>
-        <v>2.9152404184648928E-2</v>
+        <v>3.7161702846576494E-2</v>
       </c>
       <c r="L13" s="4" t="str">
         <f t="shared" ref="L13:L42" si="10">IF(D13*($B$1/100)&gt;0, (1-(1/(2.71828^(D13*($B$1/100)/169)))), "&lt;1%")</f>
@@ -11697,15 +11687,15 @@
       </c>
       <c r="J14" s="12">
         <f t="shared" si="8"/>
-        <v>0.45474868805571345</v>
+        <v>0.5399089336402908</v>
       </c>
       <c r="K14" s="12">
         <f t="shared" si="9"/>
-        <v>0.26703012679379212</v>
+        <v>0.32809133886401298</v>
       </c>
       <c r="L14" s="4">
         <f t="shared" si="10"/>
-        <v>7.8139060850156983E-2</v>
+        <v>9.8902615026041585E-2</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -11735,15 +11725,15 @@
       </c>
       <c r="J15" s="12">
         <f t="shared" si="8"/>
-        <v>6.4400709453971694E-2</v>
+        <v>8.1677867706266838E-2</v>
       </c>
       <c r="K15" s="12">
         <f t="shared" si="9"/>
-        <v>2.9152404184648928E-2</v>
+        <v>3.7161702846576494E-2</v>
       </c>
       <c r="L15" s="4">
         <f t="shared" si="10"/>
-        <v>7.3691583471030553E-3</v>
+        <v>9.4227740532037974E-3</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -11773,15 +11763,15 @@
       </c>
       <c r="J16" s="12">
         <f t="shared" si="8"/>
-        <v>0.82801600270475351</v>
+        <v>0.89494307387991301</v>
       </c>
       <c r="K16" s="12">
         <f t="shared" si="9"/>
-        <v>0.58834652657744901</v>
+        <v>0.67892929341060371</v>
       </c>
       <c r="L16" s="4">
         <f t="shared" si="10"/>
-        <v>0.27243149785310483</v>
+        <v>0.33442258236228806</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
@@ -11811,11 +11801,11 @@
       </c>
       <c r="J17" s="12">
         <f t="shared" si="8"/>
-        <v>0.10501352355029347</v>
+        <v>0.13238892828227111</v>
       </c>
       <c r="K17" s="12">
         <f t="shared" si="9"/>
-        <v>5.0457617525815013E-2</v>
+        <v>6.4123864164936761E-2</v>
       </c>
       <c r="L17" s="4" t="str">
         <f t="shared" si="10"/>
@@ -11849,15 +11839,15 @@
       </c>
       <c r="J18" s="12">
         <f t="shared" si="8"/>
-        <v>0.46671420723255974</v>
+        <v>0.55279276843269742</v>
       </c>
       <c r="K18" s="12">
         <f t="shared" si="9"/>
-        <v>0.1930526844259034</v>
+        <v>0.24009057340511064</v>
       </c>
       <c r="L18" s="4">
         <f t="shared" si="10"/>
-        <v>7.8139060850156983E-2</v>
+        <v>9.8902615026041585E-2</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
@@ -11887,15 +11877,15 @@
       </c>
       <c r="J19" s="12">
         <f t="shared" si="8"/>
-        <v>0.69150039372546757</v>
+        <v>0.7780547238278015</v>
       </c>
       <c r="K19" s="12">
         <f t="shared" si="9"/>
-        <v>0.43837599815410178</v>
+        <v>0.52215126078808638</v>
       </c>
       <c r="L19" s="4">
         <f t="shared" si="10"/>
-        <v>0.18102687303857068</v>
+        <v>0.22556467634084354</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
@@ -11925,15 +11915,15 @@
       </c>
       <c r="J20" s="12">
         <f t="shared" si="8"/>
-        <v>0.33422563696651553</v>
+        <v>0.40590123887194485</v>
       </c>
       <c r="K20" s="12">
         <f t="shared" si="9"/>
-        <v>9.8369263885248692E-2</v>
+        <v>0.12413585837442997</v>
       </c>
       <c r="L20" s="4">
         <f t="shared" si="10"/>
-        <v>7.3691583471030553E-3</v>
+        <v>9.4227740532037974E-3</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
@@ -11963,15 +11953,15 @@
       </c>
       <c r="J21" s="12">
         <f t="shared" si="8"/>
-        <v>0.39971737097178972</v>
+        <v>0.47965019854376145</v>
       </c>
       <c r="K21" s="12">
         <f t="shared" si="9"/>
-        <v>0.20490190865211622</v>
+        <v>0.2543440117125576</v>
       </c>
       <c r="L21" s="4">
         <f t="shared" si="10"/>
-        <v>7.8139060850156983E-2</v>
+        <v>9.8902615026041585E-2</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
@@ -12001,15 +11991,15 @@
       </c>
       <c r="J22" s="12">
         <f t="shared" si="8"/>
-        <v>0.36781902513495224</v>
+        <v>0.44399714713107741</v>
       </c>
       <c r="K22" s="12">
         <f t="shared" si="9"/>
-        <v>0.15643492295654537</v>
+        <v>0.19567457386278631</v>
       </c>
       <c r="L22" s="4">
         <f t="shared" si="10"/>
-        <v>2.9152404184648928E-2</v>
+        <v>3.7161702846576494E-2</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
@@ -12039,15 +12029,15 @@
       </c>
       <c r="J23" s="12">
         <f t="shared" si="8"/>
-        <v>0.54004503503167323</v>
+        <v>0.62993705698830182</v>
       </c>
       <c r="K23" s="12">
         <f t="shared" si="9"/>
-        <v>0.30914287105826299</v>
+        <v>0.37710197828213798</v>
       </c>
       <c r="L23" s="4">
         <f t="shared" si="10"/>
-        <v>0.10501352355029347</v>
+        <v>0.13238892828227111</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
@@ -12077,15 +12067,15 @@
       </c>
       <c r="J24" s="12">
         <f t="shared" si="8"/>
-        <v>0.67026524133586307</v>
+        <v>0.75831435575026795</v>
       </c>
       <c r="K24" s="12">
         <f t="shared" si="9"/>
-        <v>0.30401404031397616</v>
+        <v>0.37117671858194146</v>
       </c>
       <c r="L24" s="4">
         <f t="shared" si="10"/>
-        <v>9.8369263885248692E-2</v>
+        <v>0.12413585837442997</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -12115,15 +12105,15 @@
       </c>
       <c r="J25" s="12">
         <f t="shared" si="8"/>
-        <v>0.52623360561341148</v>
+        <v>0.61565410920424724</v>
       </c>
       <c r="K25" s="12">
         <f t="shared" si="9"/>
-        <v>0.27779306535378978</v>
+        <v>0.34069416798360319</v>
       </c>
       <c r="L25" s="4">
         <f t="shared" si="10"/>
-        <v>8.4932400084761439E-2</v>
+        <v>0.10739345208458406</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -12153,15 +12143,15 @@
       </c>
       <c r="J26" s="12">
         <f t="shared" si="8"/>
-        <v>0.41721705279824384</v>
+        <v>0.49898728324175334</v>
       </c>
       <c r="K26" s="12">
         <f t="shared" si="9"/>
-        <v>0.13110453105155007</v>
+        <v>0.16463083311584525</v>
       </c>
       <c r="L26" s="4">
         <f t="shared" si="10"/>
-        <v>4.340834212541933E-2</v>
+        <v>5.5221429161617874E-2</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -12191,15 +12181,15 @@
       </c>
       <c r="J27" s="12">
         <f t="shared" si="8"/>
-        <v>0.8148130452913559</v>
+        <v>0.8845108196096465</v>
       </c>
       <c r="K27" s="12">
         <f t="shared" si="9"/>
-        <v>0.51917313810755417</v>
+        <v>0.60830722199455689</v>
       </c>
       <c r="L27" s="4">
         <f t="shared" si="10"/>
-        <v>0.1930526844259034</v>
+        <v>0.24009057340511064</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -12229,15 +12219,15 @@
       </c>
       <c r="J28" s="12">
         <f t="shared" si="8"/>
-        <v>0.4041409487181139</v>
+        <v>0.48455333715151305</v>
       </c>
       <c r="K28" s="12">
         <f t="shared" si="9"/>
-        <v>0.22808092957753268</v>
+        <v>0.28205385797506577</v>
       </c>
       <c r="L28" s="4">
         <f t="shared" si="10"/>
-        <v>9.1675678126840299E-2</v>
+        <v>0.11580428190400116</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -12267,15 +12257,15 @@
       </c>
       <c r="J29" s="12">
         <f t="shared" si="8"/>
-        <v>0.38169221243827423</v>
+        <v>0.45956677980651262</v>
       </c>
       <c r="K29" s="12">
         <f t="shared" si="9"/>
-        <v>0.16265128758536473</v>
+        <v>0.20325355061852413</v>
       </c>
       <c r="L29" s="4">
         <f t="shared" si="10"/>
-        <v>6.4400709453971694E-2</v>
+        <v>8.1677867706266838E-2</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -12305,11 +12295,11 @@
       </c>
       <c r="J30" s="12">
         <f t="shared" si="8"/>
-        <v>2.9152404184648928E-2</v>
+        <v>3.7161702846576494E-2</v>
       </c>
       <c r="K30" s="12">
         <f t="shared" si="9"/>
-        <v>7.3691583471030553E-3</v>
+        <v>9.4227740532037974E-3</v>
       </c>
       <c r="L30" s="4" t="str">
         <f t="shared" si="10"/>
@@ -12343,15 +12333,15 @@
       </c>
       <c r="J31" s="12">
         <f t="shared" si="8"/>
-        <v>0.48607607257608232</v>
+        <v>0.57346908646631989</v>
       </c>
       <c r="K31" s="12">
         <f t="shared" si="9"/>
-        <v>0.28839796079267044</v>
+        <v>0.35306060886918966</v>
       </c>
       <c r="L31" s="4">
         <f t="shared" si="10"/>
-        <v>0.11815551588883388</v>
+        <v>0.14866250043810003</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -12381,15 +12371,15 @@
       </c>
       <c r="J32" s="12">
         <f t="shared" si="8"/>
-        <v>0.30401404031397616</v>
+        <v>0.37117671858194146</v>
       </c>
       <c r="K32" s="12">
         <f t="shared" si="9"/>
-        <v>0.18102687303857068</v>
+        <v>0.22556467634084354</v>
       </c>
       <c r="L32" s="4">
         <f t="shared" si="10"/>
-        <v>7.8139060850156983E-2</v>
+        <v>9.8902615026041585E-2</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -12419,15 +12409,15 @@
       </c>
       <c r="J33" s="12">
         <f t="shared" si="8"/>
-        <v>0.42577464470459248</v>
+        <v>0.50838465824413892</v>
       </c>
       <c r="K33" s="12">
         <f t="shared" si="9"/>
-        <v>0.25058422631632693</v>
+        <v>0.30873395916484248</v>
       </c>
       <c r="L33" s="4">
         <f t="shared" si="10"/>
-        <v>0.10501352355029347</v>
+        <v>0.13238892828227111</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -12457,15 +12447,15 @@
       </c>
       <c r="J34" s="12">
         <f t="shared" si="8"/>
-        <v>0.47841714354892473</v>
+        <v>0.56531581986916657</v>
       </c>
       <c r="K34" s="12">
         <f t="shared" si="9"/>
-        <v>0.11815551588883388</v>
+        <v>0.14866250043810003</v>
       </c>
       <c r="L34" s="4">
         <f t="shared" si="10"/>
-        <v>3.6306733849116646E-2</v>
+        <v>4.6234310570424819E-2</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -12495,15 +12485,15 @@
       </c>
       <c r="J35" s="12">
         <f t="shared" si="8"/>
-        <v>0.34883602988775952</v>
+        <v>0.42253766337222631</v>
       </c>
       <c r="K35" s="12">
         <f t="shared" si="9"/>
-        <v>0.1930526844259034</v>
+        <v>0.24009057340511064</v>
       </c>
       <c r="L35" s="4">
         <f t="shared" si="10"/>
-        <v>9.8369263885248692E-2</v>
+        <v>0.12413585837442997</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -12533,15 +12523,15 @@
       </c>
       <c r="J36" s="12">
         <f t="shared" si="8"/>
-        <v>0.46671420723255974</v>
+        <v>0.55279276843269742</v>
       </c>
       <c r="K36" s="12">
         <f t="shared" si="9"/>
-        <v>0.11815551588883388</v>
+        <v>0.14866250043810003</v>
       </c>
       <c r="L36" s="4">
         <f t="shared" si="10"/>
-        <v>1.4684012199461582E-2</v>
+        <v>1.8756759435549886E-2</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -12571,15 +12561,15 @@
       </c>
       <c r="J37" s="12">
         <f t="shared" si="8"/>
-        <v>0.38624862043206354</v>
+        <v>0.46465915993124107</v>
       </c>
       <c r="K37" s="12">
         <f t="shared" si="9"/>
-        <v>0.23376932343862444</v>
+        <v>0.28881890225373608</v>
       </c>
       <c r="L37" s="4">
         <f t="shared" si="10"/>
-        <v>9.1675678126840299E-2</v>
+        <v>0.11580428190400116</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -12609,15 +12599,15 @@
       </c>
       <c r="J38" s="12">
         <f t="shared" si="8"/>
-        <v>0.33422563696651553</v>
+        <v>0.40590123887194485</v>
       </c>
       <c r="K38" s="12">
         <f t="shared" si="9"/>
-        <v>0.1870620156931716</v>
+        <v>0.23286200541450353</v>
       </c>
       <c r="L38" s="4">
         <f t="shared" si="10"/>
-        <v>9.1675678126840299E-2</v>
+        <v>0.11580428190400116</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -12647,15 +12637,15 @@
       </c>
       <c r="J39" s="12">
         <f t="shared" si="8"/>
-        <v>0.23376932343862444</v>
+        <v>0.28881890225373608</v>
       </c>
       <c r="K39" s="12">
         <f t="shared" si="9"/>
-        <v>6.4400709453971694E-2</v>
+        <v>8.1677867706266838E-2</v>
       </c>
       <c r="L39" s="4">
         <f t="shared" si="10"/>
-        <v>7.3691583471030553E-3</v>
+        <v>9.4227740532037974E-3</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -12685,15 +12675,15 @@
       </c>
       <c r="J40" s="12">
         <f t="shared" si="8"/>
-        <v>0.48986325937563424</v>
+        <v>0.57748819089125425</v>
       </c>
       <c r="K40" s="12">
         <f t="shared" si="9"/>
-        <v>0.25610678982041879</v>
+        <v>0.3152476028782849</v>
       </c>
       <c r="L40" s="4">
         <f t="shared" si="10"/>
-        <v>0.12465396752976854</v>
+        <v>0.15668446133949132</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -12723,15 +12713,15 @@
       </c>
       <c r="J41" s="12">
         <f t="shared" si="8"/>
-        <v>0.46275516497207569</v>
+        <v>0.54853875109044536</v>
       </c>
       <c r="K41" s="12">
         <f t="shared" si="9"/>
-        <v>0.26158865667956688</v>
+        <v>0.32169986999875255</v>
       </c>
       <c r="L41" s="4">
         <f t="shared" si="10"/>
-        <v>0.13110453105155007</v>
+        <v>0.16463083311584525</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -12761,15 +12751,15 @@
       </c>
       <c r="J42" s="12">
         <f t="shared" si="8"/>
-        <v>0.41289055029629673</v>
+        <v>0.49422144620841901</v>
       </c>
       <c r="K42" s="12">
         <f t="shared" si="9"/>
-        <v>0.23941579862461304</v>
+        <v>0.29552020104870858</v>
       </c>
       <c r="L42" s="4">
         <f t="shared" si="10"/>
-        <v>0.10501352355029347</v>
+        <v>0.13238892828227111</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>